<commit_message>
modifiche odd e matrice
</commit_message>
<xml_diff>
--- a/Documentazione/Matrice di tracciabilità/TS_matrice_tracciabilità_v1.0.xlsx
+++ b/Documentazione/Matrice di tracciabilità/TS_matrice_tracciabilità_v1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\TutoratoSmart\Documentazione\Matrice di tracciabilità\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20272008-AB41-4F77-84FB-93316BEE2345}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C00C3C4-FE24-4F67-ACFF-670034CD861B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="229">
   <si>
     <t>ID</t>
   </si>
@@ -430,9 +430,6 @@
     <t>Statechart</t>
   </si>
   <si>
-    <t xml:space="preserve">ServletStudent </t>
-  </si>
-  <si>
     <t>TutoratoSmart</t>
   </si>
   <si>
@@ -604,9 +601,6 @@
     <t>Modifica attività lavorativa</t>
   </si>
   <si>
-    <t>Il sistema dovrà permettere ai tutor la visualizzazione del proprio registro di tutorato, contente le informazioni relative alle attività svolte e lo stato di quest’ultime</t>
-  </si>
-  <si>
     <t>Visualizzazione registro</t>
   </si>
   <si>
@@ -814,39 +808,6 @@
     <t>TC_8.0</t>
   </si>
   <si>
-    <t>register.jsp</t>
-  </si>
-  <si>
-    <t>request.jsp</t>
-  </si>
-  <si>
-    <t>requestInfo.jsp</t>
-  </si>
-  <si>
-    <t>requestModify.jsp</t>
-  </si>
-  <si>
-    <t>appointmentModify.jsp</t>
-  </si>
-  <si>
-    <t>activity.jsp</t>
-  </si>
-  <si>
-    <t>activityInfo.jsp</t>
-  </si>
-  <si>
-    <t>activityModifyj.java</t>
-  </si>
-  <si>
-    <t>calendar.jsp</t>
-  </si>
-  <si>
-    <t>searchTutors.jsp</t>
-  </si>
-  <si>
-    <t>searchStudents.jsp</t>
-  </si>
-  <si>
     <t>RF_TCM_1</t>
   </si>
   <si>
@@ -911,6 +872,66 @@
   </si>
   <si>
     <t>UI_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registration.jsp                           /                    RegistrationServlet                                                 </t>
+  </si>
+  <si>
+    <t>student/request.jsp                                     /                                                    RequestServlet</t>
+  </si>
+  <si>
+    <t>student/requestInfo.jsp                              /                           RequestServlet</t>
+  </si>
+  <si>
+    <t>student/requestModify.jsp                                           /                            RequestServlet</t>
+  </si>
+  <si>
+    <t>tutor/requestInfo.jsp                              /                           ShowRequestServlet</t>
+  </si>
+  <si>
+    <t>tutor/appointmentInfo.jsp                                                   /                                              ShowAppointmentServlet</t>
+  </si>
+  <si>
+    <t>tutor/appointmentInfo.jsp,appointmentModify.jsp,                                                   /                                     AppointmentServlet</t>
+  </si>
+  <si>
+    <t>tutor/activity.jsp                               /                          ActivityServlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tutor/activityInfo.jsp                  /                     ShowActivityServlet               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tutor/activityModifyj.jsp/                   ActivityServlet                                           </t>
+  </si>
+  <si>
+    <t>Il sistema dovrà permettere ai tutor la visualizzazione del proprio registro di tutorato, contenente le informazioni relative alle attività svolte e lo stato di quest’ultime</t>
+  </si>
+  <si>
+    <t>tutor/register.jsp</t>
+  </si>
+  <si>
+    <t>commission/searchTutors.jsp                                           /                          TutorsServlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commission/register.jsp                                                   /          ShowRegisterServlet  </t>
+  </si>
+  <si>
+    <t>commission/activityInfo.jsp                                       /          ShowActivityServlet</t>
+  </si>
+  <si>
+    <t>commission/activityInfo.jsp                                       /                    ActivityServlet</t>
+  </si>
+  <si>
+    <t>commission/tutorRegistration.jsp                                  /                  RegistrationServlet</t>
+  </si>
+  <si>
+    <t>commission/searchStudents.jsp,studentsList.jsp                                            /                       StudentsServlet</t>
+  </si>
+  <si>
+    <t>tutor/calendar.jsp                / Calendar,CalendarEvent</t>
+  </si>
+  <si>
+    <t>tutor/appointmentInfo.jsp                                                /            AppointmentServlet</t>
   </si>
 </sst>
 </file>
@@ -2090,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CM43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -2121,7 +2142,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="49"/>
       <c r="D1" s="17"/>
@@ -2141,10 +2162,10 @@
     </row>
     <row r="2" spans="1:91" s="18" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>64</v>
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="17"/>
@@ -2167,7 +2188,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="24"/>
@@ -2384,25 +2405,25 @@
     </row>
     <row r="5" spans="1:91" s="14" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="C5" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="D5" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="G5" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="N5" s="14" t="s">
+      <c r="P5" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="P5" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="Q5" s="14" t="s">
         <v>38</v>
@@ -2484,48 +2505,48 @@
     </row>
     <row r="6" spans="1:91" s="30" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>93</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>94</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="15" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="O6" s="16"/>
       <c r="P6" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q6" s="15" t="s">
         <v>38</v>
@@ -2533,16 +2554,16 @@
     </row>
     <row r="7" spans="1:91" ht="49.5" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>97</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>98</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>39</v>
@@ -2551,7 +2572,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="H7" s="25" t="s">
         <v>25</v>
@@ -2560,23 +2581,23 @@
         <v>46</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O7" s="26"/>
       <c r="P7" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q7" s="26" t="s">
         <v>38</v>
@@ -2584,16 +2605,16 @@
     </row>
     <row r="8" spans="1:91" ht="49.5" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>99</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>100</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>39</v>
@@ -2609,21 +2630,21 @@
         <v>47</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="26"/>
       <c r="P8" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q8" s="26" t="s">
         <v>38</v>
@@ -2631,16 +2652,16 @@
     </row>
     <row r="9" spans="1:91" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>101</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>102</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>39</v>
@@ -2649,7 +2670,7 @@
         <v>14</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>27</v>
@@ -2658,23 +2679,23 @@
         <v>48</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L9" s="25" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="O9" s="27"/>
       <c r="P9" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q9" s="26" t="s">
         <v>38</v>
@@ -2682,16 +2703,16 @@
     </row>
     <row r="10" spans="1:91" ht="49.5" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>103</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>104</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>39</v>
@@ -2707,16 +2728,16 @@
         <v>49</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>61</v>
+        <v>213</v>
       </c>
       <c r="N10" s="15"/>
       <c r="O10" s="27"/>
@@ -2727,16 +2748,16 @@
     </row>
     <row r="11" spans="1:91" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>40</v>
@@ -2745,7 +2766,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="H11" s="25" t="s">
         <v>29</v>
@@ -2754,21 +2775,23 @@
         <v>50</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="M11" s="25"/>
+        <v>193</v>
+      </c>
+      <c r="M11" s="25" t="s">
+        <v>213</v>
+      </c>
       <c r="N11" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="O11" s="27"/>
       <c r="P11" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q11" s="26" t="s">
         <v>38</v>
@@ -2776,65 +2799,67 @@
     </row>
     <row r="12" spans="1:91" ht="66" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>107</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>108</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L12" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="M12" s="25"/>
+        <v>193</v>
+      </c>
+      <c r="M12" s="25" t="s">
+        <v>228</v>
+      </c>
       <c r="N12" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O12" s="27"/>
       <c r="P12" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q12" s="26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:91" ht="49.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:91" ht="82.5" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>109</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>110</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>39</v>
@@ -2850,13 +2875,15 @@
         <v>51</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K13" s="25"/>
       <c r="L13" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="M13" s="25"/>
+        <v>194</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>214</v>
+      </c>
       <c r="N13" s="15"/>
       <c r="O13" s="27"/>
       <c r="P13" s="26"/>
@@ -2864,18 +2891,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:91" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:91" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>111</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>112</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>39</v>
@@ -2891,23 +2918,23 @@
         <v>52</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="M14" s="25" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="O14" s="27"/>
       <c r="P14" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q14" s="26" t="s">
         <v>38</v>
@@ -2915,16 +2942,16 @@
     </row>
     <row r="15" spans="1:91" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>113</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>114</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>39</v>
@@ -2933,7 +2960,7 @@
         <v>19</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="H15" s="25" t="s">
         <v>32</v>
@@ -2942,23 +2969,23 @@
         <v>53</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K15" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="M15" s="25" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="O15" s="27"/>
       <c r="P15" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q15" s="26" t="s">
         <v>38</v>
@@ -2966,16 +2993,16 @@
     </row>
     <row r="16" spans="1:91" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>115</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>116</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>40</v>
@@ -2991,14 +3018,14 @@
         <v>54</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="M16" s="25" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="N16" s="15"/>
       <c r="O16" s="27"/>
@@ -3009,16 +3036,16 @@
     </row>
     <row r="17" spans="1:17" ht="66" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>118</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>40</v>
@@ -3034,21 +3061,21 @@
         <v>55</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="25" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="M17" s="25" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="O17" s="27"/>
       <c r="P17" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q17" s="26" t="s">
         <v>38</v>
@@ -3056,16 +3083,16 @@
     </row>
     <row r="18" spans="1:17" ht="66" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>119</v>
+        <v>219</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>40</v>
@@ -3081,14 +3108,14 @@
         <v>56</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="25" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="M18" s="25" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="N18" s="15"/>
       <c r="O18" s="27"/>
@@ -3099,22 +3126,22 @@
     </row>
     <row r="19" spans="1:17" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25" t="s">
@@ -3124,13 +3151,15 @@
         <v>57</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K19" s="25"/>
       <c r="L19" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="M19" s="25"/>
+        <v>195</v>
+      </c>
+      <c r="M19" s="25" t="s">
+        <v>220</v>
+      </c>
       <c r="N19" s="15"/>
       <c r="O19" s="27"/>
       <c r="P19" s="26"/>
@@ -3140,39 +3169,39 @@
     </row>
     <row r="20" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="25" t="s">
         <v>42</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="M20" s="25" t="s">
-        <v>197</v>
+        <v>227</v>
       </c>
       <c r="N20" s="15"/>
       <c r="O20" s="27"/>
@@ -3183,41 +3212,41 @@
     </row>
     <row r="21" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="K21" s="25"/>
       <c r="L21" s="25" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="M21" s="25" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="N21" s="15"/>
       <c r="O21" s="27"/>
@@ -3228,22 +3257,22 @@
     </row>
     <row r="22" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G22" s="25"/>
       <c r="H22" s="25" t="s">
@@ -3253,16 +3282,16 @@
         <v>58</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="M22" s="25" t="s">
-        <v>189</v>
+        <v>222</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="27"/>
@@ -3273,41 +3302,41 @@
     </row>
     <row r="23" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G23" s="25"/>
       <c r="H23" s="25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="M23" s="25" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="27"/>
@@ -3318,42 +3347,44 @@
     </row>
     <row r="24" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I24" s="25" t="s">
         <v>59</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="M24" s="25"/>
+        <v>196</v>
+      </c>
+      <c r="M24" s="25" t="s">
+        <v>224</v>
+      </c>
       <c r="N24" s="15"/>
       <c r="O24" s="27"/>
       <c r="P24" s="26"/>
@@ -3363,90 +3394,90 @@
     </row>
     <row r="25" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K25" s="25"/>
       <c r="L25" s="25" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="M25" s="25" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="O25" s="27"/>
       <c r="P25" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q25" s="26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K26" s="25"/>
       <c r="L26" s="25" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="N26" s="15"/>
       <c r="O26" s="27"/>

</xml_diff>

<commit_message>
Correzione finale documentazione, matrice di tracciabilità, manuali
</commit_message>
<xml_diff>
--- a/Documentazione/Matrice di tracciabilità/TS_matrice_tracciabilità_v1.0.xlsx
+++ b/Documentazione/Matrice di tracciabilità/TS_matrice_tracciabilità_v1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\TutoratoSmart\Documentazione\Matrice di tracciabilità\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\TutoratoSmart\Documentazione\Matrice di tracciabilità\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C00C3C4-FE24-4F67-ACFF-670034CD861B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972E3A4C-DE8C-48AF-9F8A-6AE654B75B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement_Traceability_Matrix" sheetId="2" r:id="rId1"/>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="230">
   <si>
     <t>ID</t>
   </si>
@@ -274,9 +274,6 @@
 Comments</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -358,9 +355,6 @@
     <t>Test Case</t>
   </si>
   <si>
-    <t>Log</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
@@ -436,12 +430,6 @@
     <t>Project Component Name:</t>
   </si>
   <si>
-    <t>Marco Delle Cave, Manuel Pisciotta, Francesco Pagano, Alessia Oliviero</t>
-  </si>
-  <si>
-    <t>Software per supportare l'attività di tutorato dal lato studente,tutor e commissione tutorato</t>
-  </si>
-  <si>
     <t>RF_ST_1</t>
   </si>
   <si>
@@ -823,24 +811,6 @@
     <t>OD_UC16</t>
   </si>
   <si>
-    <t>GUI  STUDENT, RICHIESTA TUTORATO</t>
-  </si>
-  <si>
-    <t>GUI TUTOR, GESTIONE RICHIESTE</t>
-  </si>
-  <si>
-    <t>GUI TUTOR, GESTIONE ATTIVITA' TUTOR</t>
-  </si>
-  <si>
-    <t>GUI TUTOR,GESTIONE ATTIVITA' TUTOR</t>
-  </si>
-  <si>
-    <t>GUI COMMISSION,SUPERVISIONE TUTORATO</t>
-  </si>
-  <si>
-    <t>GUI  COMMISSION,SUPERVISIONE TUTORATO</t>
-  </si>
-  <si>
     <t>TC_10.0</t>
   </si>
   <si>
@@ -874,64 +844,97 @@
     <t>UI_10</t>
   </si>
   <si>
-    <t xml:space="preserve">registration.jsp                           /                    RegistrationServlet                                                 </t>
-  </si>
-  <si>
-    <t>student/request.jsp                                     /                                                    RequestServlet</t>
-  </si>
-  <si>
-    <t>student/requestInfo.jsp                              /                           RequestServlet</t>
-  </si>
-  <si>
-    <t>student/requestModify.jsp                                           /                            RequestServlet</t>
-  </si>
-  <si>
-    <t>tutor/requestInfo.jsp                              /                           ShowRequestServlet</t>
-  </si>
-  <si>
-    <t>tutor/appointmentInfo.jsp                                                   /                                              ShowAppointmentServlet</t>
-  </si>
-  <si>
-    <t>tutor/appointmentInfo.jsp,appointmentModify.jsp,                                                   /                                     AppointmentServlet</t>
-  </si>
-  <si>
-    <t>tutor/activity.jsp                               /                          ActivityServlet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tutor/activityInfo.jsp                  /                     ShowActivityServlet               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tutor/activityModifyj.jsp/                   ActivityServlet                                           </t>
-  </si>
-  <si>
     <t>Il sistema dovrà permettere ai tutor la visualizzazione del proprio registro di tutorato, contenente le informazioni relative alle attività svolte e lo stato di quest’ultime</t>
   </si>
   <si>
-    <t>tutor/register.jsp</t>
-  </si>
-  <si>
-    <t>commission/searchTutors.jsp                                           /                          TutorsServlet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commission/register.jsp                                                   /          ShowRegisterServlet  </t>
-  </si>
-  <si>
-    <t>commission/activityInfo.jsp                                       /          ShowActivityServlet</t>
-  </si>
-  <si>
-    <t>commission/activityInfo.jsp                                       /                    ActivityServlet</t>
-  </si>
-  <si>
-    <t>commission/tutorRegistration.jsp                                  /                  RegistrationServlet</t>
-  </si>
-  <si>
-    <t>commission/searchStudents.jsp,studentsList.jsp                                            /                       StudentsServlet</t>
-  </si>
-  <si>
-    <t>tutor/calendar.jsp                / Calendar,CalendarEvent</t>
-  </si>
-  <si>
-    <t>tutor/appointmentInfo.jsp                                                /            AppointmentServlet</t>
+    <t>Marco Delle Cave, Alessia Olivieri,Francesco Pagano, Manuel Pisciotta</t>
+  </si>
+  <si>
+    <t>Applicazione web per la gestione dell'attività di tutorato, sviluppata per il Dipartimento di Psicologia dell'Università degli Studi della Campania Luigi Vanvitelli per il corso di Ingegneria del Software 2019/2020</t>
+  </si>
+  <si>
+    <t>Student, Tutoring_Request</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Tutor, Request_Management</t>
+  </si>
+  <si>
+    <t>Tutor, Tutoring_Activity_Management</t>
+  </si>
+  <si>
+    <t>Commission, Tutoring_Supervision</t>
+  </si>
+  <si>
+    <t>View/commission/tutorRegistration.jsp                                  /                  Tutoring_Supervision/RegistrationServlet</t>
+  </si>
+  <si>
+    <t>View/commission/searchStudents.jsp,studentsList.jsp                                            /                      Tutoring_Supervision/ StudentsServlet</t>
+  </si>
+  <si>
+    <t>View/tutor/register.jsp</t>
+  </si>
+  <si>
+    <t>View/tutor/register.jsp                           /                          Tutoring_Activity_Management/ShowRegisterServlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registration.jsp                           /                    User/RegistrationServlet                                                 </t>
+  </si>
+  <si>
+    <t>View/student/request.jsp                                     /                                                   Tutoring_Request/RequestServlet</t>
+  </si>
+  <si>
+    <t>View/student/requestInfo.jsp                              /                          Tutoring_Request/ShowRequestServlet</t>
+  </si>
+  <si>
+    <t>View/tutor/requestInfo.jsp                              /                           Request_Management/ShowRequestServlet</t>
+  </si>
+  <si>
+    <t>View/tutor/requestInfo.jsp                              /                           Request_Management/RequestServlet</t>
+  </si>
+  <si>
+    <t>View/tutor/appointmentInfo.jsp                                       /                       Request_Management/AppointmentServlet</t>
+  </si>
+  <si>
+    <t>View/tutor/appointmentInfo.jsp                                                   /                                              Request_Management/ShowAppointmentServlet</t>
+  </si>
+  <si>
+    <t>View/tutor/activity.jsp                               /                          Tutoring_Activity_Management/ActivityServlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View/tutor/activityInfo.jsp                  /                     Tutoring_Activity_Management/ShowActivityServlet               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">View/tutor/activityModifyj.jsp                                /                        Tutoring_Activity_Management/ActivityServlet                                           </t>
+  </si>
+  <si>
+    <t>View/commission/searchTutors.jsp                                           /                          Tutoring_Supervision/TutorsServlet</t>
+  </si>
+  <si>
+    <t>View/tutor/calendar.jsp                /                                                         Request_Management/CalendarServlet</t>
+  </si>
+  <si>
+    <t>View/commission/activityInfo.jsp                                       /                    Tutoring_Supervision/ActivityServlet</t>
+  </si>
+  <si>
+    <t>View/commission/activityInfo.jsp                                       /          Tutoring_Supervision/ShowActivityServlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View/commission/register.jsp                                                   /          Tutoring_Supervision/ShowRegisterServlet  </t>
+  </si>
+  <si>
+    <t>Il file viene generato tramite script Javascript, usando la libreria jsPdf.</t>
+  </si>
+  <si>
+    <t>View/tutor/appointmentInfo.jsp, View/tutor/appointmentModify.jsp,                                                   /                                    Request_Management/ShowAppointmentServlet, Request_Management/AppointmentServlet</t>
+  </si>
+  <si>
+    <t>View/student/requestInfo.jsp, View/student/requestModify.jsp                                           /                            Tutoring_Request/ShowRequestServlet, Tutoring_Request/RequestServlet</t>
   </si>
 </sst>
 </file>
@@ -2111,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CM43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -2121,7 +2124,7 @@
     <col min="2" max="2" width="37.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="52.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" style="3" customWidth="1"/>
@@ -2129,7 +2132,7 @@
     <col min="10" max="10" width="23.7109375" style="3" customWidth="1"/>
     <col min="11" max="11" width="18" style="3" customWidth="1"/>
     <col min="12" max="12" width="24.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="23.28515625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="49.28515625" style="4" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" style="4" customWidth="1"/>
     <col min="15" max="15" width="43" style="4" customWidth="1"/>
     <col min="16" max="16" width="68.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -2142,7 +2145,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="49"/>
       <c r="D1" s="17"/>
@@ -2162,10 +2165,10 @@
     </row>
     <row r="2" spans="1:91" s="18" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>63</v>
+        <v>200</v>
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="17"/>
@@ -2188,7 +2191,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>64</v>
+        <v>201</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="24"/>
@@ -2289,28 +2292,28 @@
         <v>5</v>
       </c>
       <c r="D4" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>24</v>
-      </c>
       <c r="I4" s="34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J4" s="34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K4" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L4" s="34" t="s">
         <v>7</v>
@@ -2319,11 +2322,9 @@
         <v>6</v>
       </c>
       <c r="N4" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="35" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="O4" s="35"/>
       <c r="P4" s="31" t="s">
         <v>4</v>
       </c>
@@ -2405,28 +2406,31 @@
     </row>
     <row r="5" spans="1:91" s="14" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="P5" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="P5" s="14" t="s">
-        <v>90</v>
-      </c>
       <c r="Q5" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
@@ -2505,882 +2509,874 @@
     </row>
     <row r="6" spans="1:91" s="30" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>144</v>
-      </c>
       <c r="I6" s="25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="15" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="O6" s="16"/>
       <c r="P6" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:91" ht="49.5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:91" ht="82.5" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="K7" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="N7" s="15" t="s">
         <v>176</v>
-      </c>
-      <c r="L7" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="M7" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="N7" s="15" t="s">
-        <v>180</v>
       </c>
       <c r="O7" s="26"/>
       <c r="P7" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q7" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:91" ht="49.5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:91" ht="82.5" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="26"/>
       <c r="P8" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:91" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="L9" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="K9" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>192</v>
-      </c>
       <c r="M9" s="25" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O9" s="27"/>
       <c r="P9" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q9" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:91" ht="99" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="Q9" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:91" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>94</v>
-      </c>
       <c r="C10" s="25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="N10" s="15"/>
       <c r="O10" s="27"/>
       <c r="P10" s="26"/>
       <c r="Q10" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:91" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="M11" s="25" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="O11" s="27"/>
       <c r="P11" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q11" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:91" ht="99" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="Q11" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:91" ht="66" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>94</v>
-      </c>
       <c r="C12" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="G12" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>145</v>
-      </c>
       <c r="I12" s="25" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="K12" s="25" t="s">
-        <v>177</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="K12" s="25"/>
       <c r="L12" s="25" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="O12" s="27"/>
       <c r="P12" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q12" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:91" ht="99" x14ac:dyDescent="0.2">
+      <c r="A13" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="Q12" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:91" ht="82.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>94</v>
-      </c>
       <c r="C13" s="25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K13" s="25"/>
       <c r="L13" s="25" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="M13" s="25" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="N13" s="15"/>
       <c r="O13" s="27"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:91" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="K14" s="25" t="s">
-        <v>177</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="K14" s="25"/>
       <c r="L14" s="25" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="M14" s="25" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="O14" s="27"/>
       <c r="P14" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:91" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="K15" s="25" t="s">
-        <v>177</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="K15" s="25"/>
       <c r="L15" s="25" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="M15" s="25" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="O15" s="27"/>
       <c r="P15" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q15" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:91" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="M16" s="25" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N16" s="15"/>
       <c r="O16" s="27"/>
       <c r="P16" s="26"/>
       <c r="Q16" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="99" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" ht="66" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>40</v>
-      </c>
       <c r="F17" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="25" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="M17" s="25" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="O17" s="27"/>
       <c r="P17" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q17" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="82.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="Q17" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="66" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>94</v>
-      </c>
       <c r="C18" s="25" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="25"/>
       <c r="H18" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="25" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="M18" s="25" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="N18" s="15"/>
       <c r="O18" s="27"/>
       <c r="P18" s="26"/>
       <c r="Q18" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K19" s="25"/>
       <c r="L19" s="25" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="M19" s="25" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="N19" s="15"/>
       <c r="O19" s="27"/>
       <c r="P19" s="26"/>
       <c r="Q19" s="26" t="s">
-        <v>38</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>39</v>
+        <v>204</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="M20" s="25" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="N20" s="15"/>
       <c r="O20" s="27"/>
       <c r="P20" s="26"/>
       <c r="Q20" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="J21" s="25" t="s">
         <v>187</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>191</v>
       </c>
       <c r="K21" s="25"/>
       <c r="L21" s="25" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="M21" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N21" s="15"/>
       <c r="O21" s="27"/>
       <c r="P21" s="26"/>
       <c r="Q21" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G22" s="25"/>
       <c r="H22" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="M22" s="25" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="27"/>
       <c r="P22" s="26"/>
       <c r="Q22" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G23" s="25"/>
       <c r="H23" s="25" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="M23" s="25" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="27"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="M24" s="25" t="s">
         <v>224</v>
@@ -3389,101 +3385,101 @@
       <c r="O24" s="27"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K25" s="25"/>
       <c r="L25" s="25" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="M25" s="25" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="O25" s="27"/>
       <c r="P25" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q25" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K26" s="25"/>
       <c r="L26" s="25" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N26" s="15"/>
       <c r="O26" s="27"/>
       <c r="P26" s="26"/>
       <c r="Q26" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>